<commit_message>
add description likard parser
</commit_message>
<xml_diff>
--- a/urls/urls.xlsx
+++ b/urls/urls.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>instr_urls</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>https://kirov.instrument.ms/vse-dlya-sada/motobloki-i-kultivatory</t>
+  </si>
+  <si>
+    <t>https://instrument-orugie.ru/catalog/Sadovaya-tehnika/Motobloki/</t>
   </si>
 </sst>
 </file>
@@ -297,11 +300,15 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="B2"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>